<commit_message>
Revision 1 del dia 20/5/2019
</commit_message>
<xml_diff>
--- a/EjercicioPrestamo/EjercicioPrestamo.xlsx
+++ b/EjercicioPrestamo/EjercicioPrestamo.xlsx
@@ -1,58 +1,74 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\eq016\COMPARTIDO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuario\julio.martinez\Desarrollo\JAVA-TUTORIAL\curso-java\git-repos\ejercicioPrestamo\EjercicioPrestamo\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9FE60DE-158F-4EC5-98E6-777679560C8E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8205"/>
+    <workbookView xWindow="2278" yWindow="2278" windowWidth="18851" windowHeight="9844" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="capital">Hoja1!$B$1</definedName>
+    <definedName name="cuotas">Hoja1!$B$2</definedName>
+    <definedName name="diasAño">Hoja1!$F$1</definedName>
+    <definedName name="diasPeriodo">Hoja1!$F$2</definedName>
     <definedName name="razon">Hoja1!$B$6</definedName>
+    <definedName name="tasa">Hoja1!$B$3</definedName>
     <definedName name="valorcuota">Hoja1!$B$7</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Capital</t>
   </si>
   <si>
+    <t>Bigdecimal</t>
+  </si>
+  <si>
+    <t>Días año</t>
+  </si>
+  <si>
     <t>Cuotas</t>
   </si>
   <si>
+    <t>Días Periodo</t>
+  </si>
+  <si>
     <t>TNA</t>
   </si>
   <si>
-    <t>Bigdecimal</t>
-  </si>
-  <si>
     <t>Sistema</t>
   </si>
   <si>
     <t>Frances</t>
   </si>
   <si>
+    <t>RAZON</t>
+  </si>
+  <si>
     <t>VC</t>
-  </si>
-  <si>
-    <t>RAZON</t>
   </si>
   <si>
     <t>Cuota</t>
@@ -67,33 +83,33 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00&quot; €&quot;"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -133,12 +149,12 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -173,7 +189,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -185,7 +201,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -232,6 +248,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -267,6 +300,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -418,19 +468,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1048576"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" customWidth="1"/>
+    <col min="4" max="5" width="12" customWidth="1"/>
+    <col min="6" max="1025" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,175 +492,223 @@
         <v>100000</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
       </c>
       <c r="B2">
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6">
-        <f>40/365*30/100</f>
+        <f>tasa/diasAño*diasPeriodo/100</f>
         <v>3.287671232876712E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B7">
-        <f>B1*B6*(1+B6)^6/((1+B6)^6-1)</f>
+        <f>capital*razon*(1+razon)^cuotas/((1+razon)^cuotas-1)</f>
         <v>18636.139008372757</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="2" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="E9" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
         <v>1</v>
       </c>
-      <c r="B10" s="4">
-        <f>valorcuota</f>
+      <c r="B10" s="3">
+        <f t="shared" ref="B10:B15" si="0">valorcuota</f>
         <v>18636.139008372757</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <f>capital*razon</f>
         <v>3287.6712328767121</v>
       </c>
-      <c r="D10" s="4">
-        <f>B10-C10</f>
+      <c r="D10" s="3">
+        <f t="shared" ref="D10:D15" si="1">B10-C10</f>
         <v>15348.467775496045</v>
       </c>
-      <c r="E10" s="4">
-        <f>capital-B10</f>
-        <v>81363.86099162724</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="E10" s="3">
+        <f>capital-D10</f>
+        <v>84651.532224503957</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
         <v>2</v>
       </c>
-      <c r="B11" s="4">
-        <f>valorcuota</f>
+      <c r="B11" s="3">
+        <f t="shared" si="0"/>
         <v>18636.139008372757</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <f>E10*razon</f>
-        <v>2674.9762517795252</v>
-      </c>
-      <c r="D11" s="4">
-        <f>B11-C11</f>
-        <v>15961.162756593232</v>
-      </c>
-      <c r="E11" s="4">
-        <f>E10-B11</f>
-        <v>62727.72198325448</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+        <v>2783.0640731343765</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="1"/>
+        <v>15853.074935238379</v>
+      </c>
+      <c r="E11" s="3">
+        <f>E10-D11</f>
+        <v>68798.457289265585</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
         <v>3</v>
       </c>
-      <c r="B12" s="4">
-        <f>valorcuota</f>
+      <c r="B12" s="3">
+        <f t="shared" si="0"/>
         <v>18636.139008372757</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="C12" s="3">
+        <f>E11*razon</f>
+        <v>2261.8670889621558</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="1"/>
+        <v>16374.271919410601</v>
+      </c>
+      <c r="E12" s="3">
+        <f>E11-D12</f>
+        <v>52424.185369854982</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
         <v>4</v>
       </c>
-      <c r="B13" s="4">
-        <f>valorcuota</f>
+      <c r="B13" s="3">
+        <f t="shared" si="0"/>
         <v>18636.139008372757</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="C13" s="3">
+        <f>E12*razon</f>
+        <v>1723.5348614746842</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="1"/>
+        <v>16912.604146898073</v>
+      </c>
+      <c r="E13" s="3">
+        <f>E12-D13</f>
+        <v>35511.581222956913</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
         <v>5</v>
       </c>
-      <c r="B14" s="4">
-        <f>valorcuota</f>
+      <c r="B14" s="3">
+        <f t="shared" si="0"/>
         <v>18636.139008372757</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="C14" s="3">
+        <f>E13*razon</f>
+        <v>1167.5040402068025</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="1"/>
+        <v>17468.634968165956</v>
+      </c>
+      <c r="E14" s="3">
+        <f>E13-D14</f>
+        <v>18042.946254790957</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
         <v>6</v>
       </c>
-      <c r="B15" s="4">
-        <f>valorcuota</f>
+      <c r="B15" s="3">
+        <f t="shared" si="0"/>
         <v>18636.139008372757</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
-    </row>
-    <row r="1048576" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C15" s="3">
+        <f>E14*razon</f>
+        <v>593.19275358216839</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="1"/>
+        <v>18042.94625479059</v>
+      </c>
+      <c r="E15" s="3">
+        <f>E14-D15</f>
+        <v>3.6743585951626301E-10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="4"/>
+    </row>
+    <row r="1048576" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B1048576" t="e">
         <f>B1048570*B1048575*(1+B1048575)^6/((1+B1048575)^6-1)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>